<commit_message>
Navoiy viloyati grafa qo'shish kerak
</commit_message>
<xml_diff>
--- a/tash_obl_indeks_2022_07.xlsx
+++ b/tash_obl_indeks_2022_07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.usmonov\Desktop\consumer_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633E0F49-99CD-4132-BC5C-6D8619F41714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982016CB-4FC3-40EC-A43F-86BCABB4C855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="720" windowWidth="10695" windowHeight="12675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2945,8 +2945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AQ8" sqref="AQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2955,7 +2955,9 @@
     <col min="7" max="10" width="0" hidden="1" customWidth="1"/>
     <col min="12" max="14" width="0" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="42" width="0" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="41" width="0" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Toshkent viloyati doklad oxirgi
</commit_message>
<xml_diff>
--- a/tash_obl_indeks_2022_07.xlsx
+++ b/tash_obl_indeks_2022_07.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.usmonov\Desktop\consumer_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982016CB-4FC3-40EC-A43F-86BCABB4C855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D19EA66-C44C-466C-B73D-8089FEDADE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="720" windowWidth="10695" windowHeight="12675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="1380" windowWidth="13770" windowHeight="14055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -2033,10 +2033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J23"/>
+      <selection activeCell="B2" sqref="B2:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,674 +2080,674 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="C2">
         <v>123</v>
       </c>
       <c r="D2">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E2">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="F2">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="G2">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="H2">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I2">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="J2">
-        <v>148</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="C3">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="D3">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E3">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="F3">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="G3">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="H3">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="I3">
-        <v>115</v>
+        <v>161</v>
       </c>
       <c r="J3">
-        <v>129</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B4">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C4">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D4">
         <v>144</v>
       </c>
       <c r="E4">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="F4">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="G4">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H4">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="I4">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="J4">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C5">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D5">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E5">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="F5">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="G5">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="H5">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I5">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="J5">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B6">
+        <v>136</v>
+      </c>
+      <c r="C6">
         <v>143</v>
       </c>
-      <c r="C6">
-        <v>128</v>
-      </c>
       <c r="D6">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E6">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="F6">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G6">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="H6">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="I6">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="J6">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C7">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D7">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E7">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="F7">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G7">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H7">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I7">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J7">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C8">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="D8">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E8">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="F8">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="G8">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="H8">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I8">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="J8">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C9">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D9">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E9">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F9">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G9">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="H9">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="I9">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="J9">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B10">
+        <v>132</v>
+      </c>
+      <c r="C10">
+        <v>123</v>
+      </c>
+      <c r="D10">
         <v>134</v>
       </c>
-      <c r="C10">
-        <v>126</v>
-      </c>
-      <c r="D10">
-        <v>124</v>
-      </c>
       <c r="E10">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="F10">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G10">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H10">
+        <v>145</v>
+      </c>
+      <c r="I10">
+        <v>144</v>
+      </c>
+      <c r="J10">
         <v>148</v>
-      </c>
-      <c r="I10">
-        <v>135</v>
-      </c>
-      <c r="J10">
-        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B11">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C11">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D11">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="E11">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F11">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="G11">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H11">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="I11">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J11">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B12">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C12">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="D12">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E12">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F12">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G12">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="H12">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I12">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="J12">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C13">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D13">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E13">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="F13">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="G13">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="H13">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="I13">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="J13">
-        <v>140</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C14">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D14">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="E14">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="F14">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="G14">
+        <v>167</v>
+      </c>
+      <c r="H14">
         <v>149</v>
       </c>
-      <c r="H14">
+      <c r="I14">
+        <v>129</v>
+      </c>
+      <c r="J14">
         <v>148</v>
-      </c>
-      <c r="I14">
-        <v>142</v>
-      </c>
-      <c r="J14">
-        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E15">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F15">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G15">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H15">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="I15">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="J15">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C16">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="D16">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E16">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="F16">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="G16">
         <v>157</v>
       </c>
       <c r="H16">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="I16">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J16">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C17">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D17">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E17">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F17">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G17">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="H17">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I17">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="J17">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C18">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D18">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E18">
         <v>118</v>
       </c>
       <c r="F18">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G18">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="H18">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="I18">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="J18">
-        <v>154</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C19">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="D19">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E19">
         <v>106</v>
       </c>
       <c r="F19">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="G19">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H19">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="I19">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="J19">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B20">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C20">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D20">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E20">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="F20">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="G20">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="H20">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="I20">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="J20">
-        <v>128</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C21">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="D21">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E21">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F21">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="G21">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="H21">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="I21">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="J21">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C22">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D22">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E22">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F22">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G22">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H22">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="I22">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="J22">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2782,39 +2782,42 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>131</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>116</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>132</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>99</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>116</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>158</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>140</v>
       </c>
-      <c r="I24">
+      <c r="I25">
         <v>140</v>
       </c>
-      <c r="J24">
+      <c r="J25">
         <v>146</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J23">
+    <sortCondition descending="1" ref="B2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -2945,8 +2948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ8" sqref="AQ8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>